<commit_message>
updated lint results in folder
</commit_message>
<xml_diff>
--- a/Results/standard_tests/ErrorLogs.xlsx
+++ b/Results/standard_tests/ErrorLogs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federicaventriglia/Documents/Universita/TESI/EspressoTests/EspressoTests/Results/standard_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BC90C0-C235-5F4B-A865-46F80CF06087}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F102BB2-44DA-234D-A637-A9AFD16BDA24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="8" xr2:uid="{DDC8EAF8-2D11-8B4E-9049-155342BC85AE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="7" xr2:uid="{DDC8EAF8-2D11-8B4E-9049-155342BC85AE}"/>
   </bookViews>
   <sheets>
     <sheet name="BMI" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="257">
   <si>
     <t>NoMatchingViewException</t>
   </si>
@@ -892,12 +892,24 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="10">
     <font>
       <sz val="12"/>
@@ -970,7 +982,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1002,6 +1014,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1150,7 +1168,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -1195,18 +1213,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1254,18 +1260,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1316,15 +1310,71 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2979,25 +3029,25 @@
             <c:numRef>
               <c:f>Editor!$E$2:$J$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0.18518518518518517</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>0.18518518518518517</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>0.14814814814814814</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0.18518518518518517</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0.14814814814814814</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>0.18518518518518517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3119,7 +3169,7 @@
             <c:numRef>
               <c:f>Editor!$E$3:$J$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3259,25 +3309,25 @@
             <c:numRef>
               <c:f>Editor!$E$4:$J$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0.18518518518518517</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>0.18518518518518517</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>0.14814814814814814</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0.18518518518518517</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0.14814814814814814</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>0.18518518518518517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3374,7 +3424,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3645,25 +3695,25 @@
             <c:numRef>
               <c:f>PRIMARY!$E$2:$J$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>0.22500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>0.22500000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3785,25 +3835,25 @@
             <c:numRef>
               <c:f>PRIMARY!$E$3:$J$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3925,25 +3975,25 @@
             <c:numRef>
               <c:f>PRIMARY!$E$4:$J$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>7.4999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>7.4999999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4040,7 +4090,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4315,25 +4365,25 @@
             <c:numRef>
               <c:f>Shopping!$E$2:$J$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>0.15625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4455,22 +4505,22 @@
             <c:numRef>
               <c:f>Shopping!$E$3:$J$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -4595,25 +4645,25 @@
             <c:numRef>
               <c:f>Shopping!$E$4:$J$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4710,7 +4760,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4981,25 +5031,25 @@
             <c:numRef>
               <c:f>'simply-do'!$E$2:$J$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4.3478260869565216E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>0.21739130434782608</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>8.6956521739130432E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>4.3478260869565216E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>4.3478260869565216E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>0.39130434782608697</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5121,25 +5171,25 @@
             <c:numRef>
               <c:f>'simply-do'!$E$3:$J$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4.3478260869565216E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>4.3478260869565216E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0.13043478260869565</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>4.3478260869565216E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>4.3478260869565216E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>4.3478260869565216E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5261,13 +5311,13 @@
             <c:numRef>
               <c:f>'simply-do'!$E$4:$J$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>0.30434782608695654</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -5276,10 +5326,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>4.3478260869565216E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>0.34782608695652173</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5376,7 +5426,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5644,7 +5694,7 @@
             <c:numRef>
               <c:f>total!$B$2:$G$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>31</c:v>
@@ -5781,7 +5831,7 @@
             <c:numRef>
               <c:f>total!$B$3:$G$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>19</c:v>
@@ -5918,7 +5968,7 @@
             <c:numRef>
               <c:f>total!$B$4:$G$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
@@ -10289,15 +10339,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>264160</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>325120</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10673,23 +10723,23 @@
       <c r="C1" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="50" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="47" t="s">
         <v>116</v>
       </c>
     </row>
@@ -10703,30 +10753,30 @@
       <c r="C2" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="53">
+      <c r="E2" s="49">
         <f>COUNTIF(C1:C33,"C1")</f>
         <v>7</v>
       </c>
-      <c r="F2" s="53">
+      <c r="F2" s="49">
         <f>COUNTIF(C1:C33,"C2")</f>
         <v>2</v>
       </c>
-      <c r="G2" s="53">
+      <c r="G2" s="49">
         <f>COUNTIF(C1:C33,"C3")</f>
         <v>7</v>
       </c>
-      <c r="H2" s="53">
+      <c r="H2" s="49">
         <f>COUNTIF(C1:C33,"C4")</f>
         <v>7</v>
       </c>
-      <c r="I2" s="53">
+      <c r="I2" s="49">
         <f>COUNTIF(C1:C33,"C5")</f>
         <v>8</v>
       </c>
-      <c r="J2" s="54">
+      <c r="J2" s="50">
         <f>COUNTIF(C1:C33,"C6")</f>
         <v>2</v>
       </c>
@@ -10741,30 +10791,30 @@
       <c r="C3" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="53">
+      <c r="D3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="49">
         <f>COUNTIFS(C1:C33,"C1",A1:A33,"NoMatchingViewException")</f>
         <v>7</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="49">
         <f>COUNTIFS(C1:C33,"C2",A1:A33,"NoMatchingViewException")</f>
         <v>2</v>
       </c>
-      <c r="G3" s="53">
+      <c r="G3" s="49">
         <f>COUNTIFS(C1:C33,"C3",A1:A33,"NoMatchingViewException")</f>
         <v>7</v>
       </c>
-      <c r="H3" s="53">
+      <c r="H3" s="49">
         <f>COUNTIFS(C1:C33,"C4",A1:A33,"NoMatchingViewException")</f>
         <v>7</v>
       </c>
-      <c r="I3" s="53">
+      <c r="I3" s="49">
         <f>COUNTIFS(C1:C33,"C5",A1:A33,"NoMatchingViewException")</f>
         <v>8</v>
       </c>
-      <c r="J3" s="54">
+      <c r="J3" s="50">
         <f>COUNTIFS(C1:C33,"C6",A1:A33,"NoMatchingViewException")</f>
         <v>2</v>
       </c>
@@ -10779,30 +10829,30 @@
       <c r="C4" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="57">
+      <c r="E4" s="53">
         <f>COUNTIFS(C1:C33,"C1",A1:A33,"AmbiguousViewMatcherException")</f>
         <v>0</v>
       </c>
-      <c r="F4" s="57">
+      <c r="F4" s="53">
         <f>COUNTIFS(C1:C33,"C2",A1:A33,"AmbiguousViewMatcherException")</f>
         <v>0</v>
       </c>
-      <c r="G4" s="57">
+      <c r="G4" s="53">
         <f>COUNTIFS(C1:C33,"C3",A1:A33,"AmbiguousViewMatcherException")</f>
         <v>0</v>
       </c>
-      <c r="H4" s="57">
+      <c r="H4" s="53">
         <f>COUNTIFS(C1:C33,"C4",A1:A33,"AmbiguousViewMatcherException")</f>
         <v>0</v>
       </c>
-      <c r="I4" s="57">
+      <c r="I4" s="53">
         <f>COUNTIFS(C1:C33,"C5",A1:A33,"AmbiguousViewMatcherException")</f>
         <v>0</v>
       </c>
-      <c r="J4" s="58">
+      <c r="J4" s="54">
         <f>COUNTIFS(C1:C33,"C6",A1:A33,"AmbiguousViewMatcherException")</f>
         <v>0</v>
       </c>
@@ -11127,26 +11177,26 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="46">
+      <c r="B34" s="42">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="47">
+      <c r="B35" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="48">
+      <c r="B36" s="44">
         <v>33</v>
       </c>
     </row>
@@ -11181,23 +11231,23 @@
       <c r="C1" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="66" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="59" t="s">
         <v>116</v>
       </c>
     </row>
@@ -11211,7 +11261,7 @@
       <c r="C2" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="55" t="s">
         <v>144</v>
       </c>
       <c r="E2" s="16">
@@ -11249,7 +11299,7 @@
       <c r="C3" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="56" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="16">
@@ -11287,7 +11337,7 @@
       <c r="C4" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="57" t="s">
         <v>110</v>
       </c>
       <c r="E4" s="18">
@@ -11644,7 +11694,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -11674,7 +11724,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -11686,33 +11736,33 @@
       <c r="D2" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="38">
         <f>COUNTIF(C1:C42,"C1")</f>
         <v>7</v>
       </c>
-      <c r="F2" s="42">
+      <c r="F2" s="38">
         <f>COUNTIF(C1:C42,"C2")</f>
         <v>8</v>
       </c>
-      <c r="G2" s="42">
+      <c r="G2" s="38">
         <f>COUNTIF(C1:C42,"C3")</f>
         <v>7</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="38">
         <f>COUNTIF(C1:C42,"C4")</f>
         <v>7</v>
       </c>
-      <c r="I2" s="42">
+      <c r="I2" s="38">
         <f>COUNTIF(C1:C42,"C5")</f>
         <v>7</v>
       </c>
-      <c r="J2" s="43">
+      <c r="J2" s="39">
         <f>COUNTIF(C1:C42,"C6")</f>
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
@@ -11724,33 +11774,33 @@
       <c r="D3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="38">
         <f>COUNTIFS(C1:C42,"C1",A1:A42,"NoMatchingViewException")</f>
         <v>5</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="38">
         <f>COUNTIFS(C1:C42,"C2",A1:A42,"NoMatchingViewException")</f>
         <v>5</v>
       </c>
-      <c r="G3" s="42">
+      <c r="G3" s="38">
         <f>COUNTIFS(C1:C42,"C3",A1:A42,"NoMatchingViewException")</f>
         <v>7</v>
       </c>
-      <c r="H3" s="42">
+      <c r="H3" s="38">
         <f>COUNTIFS(C1:C42,"C4",A1:A42,"NoMatchingViewException")</f>
         <v>5</v>
       </c>
-      <c r="I3" s="42">
+      <c r="I3" s="38">
         <f>COUNTIFS(C1:C42,"C5",A1:A42,"NoMatchingViewException")</f>
         <v>7</v>
       </c>
-      <c r="J3" s="43">
+      <c r="J3" s="39">
         <f>COUNTIFS(C1:C42,"C6",A1:A42,"NoMatchingViewException")</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
@@ -11762,33 +11812,33 @@
       <c r="D4" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="40">
         <f>COUNTIFS(C1:C42,"C1",A1:A42,"AmbiguousViewMatcherException")</f>
         <v>2</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="40">
         <f>COUNTIFS(C1:C42,"C2",A1:A42,"AmbiguousViewMatcherException")</f>
         <v>3</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="40">
         <f>COUNTIFS(C1:C42,"C3",A1:A42,"AmbiguousViewMatcherException")</f>
         <v>0</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="40">
         <f>COUNTIFS(C1:C42,"C4",A1:A42,"AmbiguousViewMatcherException")</f>
         <v>2</v>
       </c>
-      <c r="I4" s="44">
+      <c r="I4" s="40">
         <f>COUNTIFS(C1:C42,"C5",A1:A42,"AmbiguousViewMatcherException")</f>
         <v>0</v>
       </c>
-      <c r="J4" s="45">
+      <c r="J4" s="41">
         <f>COUNTIFS(C1:C42,"C6",A1:A42,"AmbiguousViewMatcherException")</f>
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
@@ -11799,7 +11849,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
@@ -11810,7 +11860,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B7" t="s">
@@ -11821,7 +11871,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
@@ -11832,7 +11882,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B9" t="s">
@@ -11843,7 +11893,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
@@ -11854,7 +11904,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B11" t="s">
@@ -11865,7 +11915,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B12" t="s">
@@ -11876,7 +11926,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B13" t="s">
@@ -11887,7 +11937,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B14" t="s">
@@ -11898,7 +11948,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B15" t="s">
@@ -11909,7 +11959,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B16" t="s">
@@ -11920,7 +11970,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B17" t="s">
@@ -11931,7 +11981,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B18" t="s">
@@ -11942,7 +11992,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B19" t="s">
@@ -11953,7 +12003,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B20" t="s">
@@ -11964,7 +12014,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B21" t="s">
@@ -11975,7 +12025,7 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B22" t="s">
@@ -11986,7 +12036,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B23" t="s">
@@ -11997,7 +12047,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B24" t="s">
@@ -12008,7 +12058,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B25" t="s">
@@ -12019,7 +12069,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B26" t="s">
@@ -12030,7 +12080,7 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B27" t="s">
@@ -12041,7 +12091,7 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B28" t="s">
@@ -12052,7 +12102,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B29" t="s">
@@ -12063,7 +12113,7 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B30" t="s">
@@ -12074,7 +12124,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B31" t="s">
@@ -12085,7 +12135,7 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B32" t="s">
@@ -12096,7 +12146,7 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B33" t="s">
@@ -12107,7 +12157,7 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B34" t="s">
@@ -12118,7 +12168,7 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B35" t="s">
@@ -12129,7 +12179,7 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B36" t="s">
@@ -12140,7 +12190,7 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
@@ -12151,7 +12201,7 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B38" t="s">
@@ -12162,7 +12212,7 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B39" t="s">
@@ -12173,7 +12223,7 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B40" t="s">
@@ -12184,7 +12234,7 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B41" t="s">
@@ -12195,7 +12245,7 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B42" t="s">
@@ -12206,16 +12256,16 @@
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="38">
+      <c r="B43" s="34">
         <v>30</v>
       </c>
-      <c r="C43" s="33"/>
+      <c r="C43" s="29"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="35" t="s">
         <v>178</v>
       </c>
       <c r="B44" s="13">
@@ -12224,10 +12274,10 @@
       <c r="C44" s="11"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="41">
+      <c r="B45" s="37">
         <v>42</v>
       </c>
       <c r="C45" s="15"/>
@@ -12258,10 +12308,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE67C548-86DE-2347-9114-A4AFF6D8F949}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12314,29 +12364,29 @@
       <c r="D2" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="16">
-        <f>COUNTIF(C1:C28,"C1")</f>
-        <v>5</v>
-      </c>
-      <c r="F2" s="16">
-        <f>COUNTIF(C1:C41,"C2")</f>
-        <v>5</v>
-      </c>
-      <c r="G2" s="16">
-        <f>COUNTIF(C1:C41,"C3")</f>
-        <v>4</v>
-      </c>
-      <c r="H2" s="16">
-        <f>COUNTIF(C1:C41,"C4")</f>
-        <v>5</v>
-      </c>
-      <c r="I2" s="16">
-        <f>COUNTIF(C1:C41,"C5")</f>
-        <v>4</v>
-      </c>
-      <c r="J2" s="17">
-        <f>COUNTIF(C1:C41,"C6")</f>
-        <v>5</v>
+      <c r="E2" s="88">
+        <f>COUNTIF(C1:C28,"C1")/B33</f>
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="F2" s="88">
+        <f>COUNTIF(C1:C41,"C2")/B33</f>
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="G2" s="88">
+        <f>COUNTIF(C1:C41,"C3")/B33</f>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="H2" s="88">
+        <f>COUNTIF(C1:C41,"C4")/B33</f>
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="I2" s="88">
+        <f>COUNTIF(C1:C41,"C5")/B33</f>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="J2" s="89">
+        <f>COUNTIF(C1:C41,"C6")/B33</f>
+        <v>0.18518518518518517</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12352,28 +12402,28 @@
       <c r="D3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="16">
-        <f>COUNTIFS(C1:C28,"C1",A1:A28,"NoMatchingViewException")</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="16">
-        <f>COUNTIFS(C1:C28,"C2",A1:A28,"NoMatchingViewException")</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="16">
-        <f>COUNTIFS(C1:C28,"C3",A1:A28,"NoMatchingViewException")</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="16">
-        <f>COUNTIFS(C1:C28,"C4",A1:A28,"NoMatchingViewException")</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="16">
-        <f>COUNTIFS(C1:C28,"C5",A1:A28,"NoMatchingViewException")</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="17">
-        <f>COUNTIFS(C1:C28,"C6",A1:A28,"NoMatchingViewException")</f>
+      <c r="E3" s="88">
+        <f>COUNTIFS(C1:C28,"C1",A1:A28,"NoMatchingViewException")/B33</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="88">
+        <f>COUNTIFS(C1:C28,"C2",A1:A28,"NoMatchingViewException")/B33</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="88">
+        <f>COUNTIFS(C1:C28,"C3",A1:A28,"NoMatchingViewException")/B33</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="88">
+        <f>COUNTIFS(C1:C28,"C4",A1:A28,"NoMatchingViewException")/B33</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="88">
+        <f>COUNTIFS(C1:C28,"C5",A1:A28,"NoMatchingViewException")/B33</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="89">
+        <f>COUNTIFS(C1:C28,"C6",A1:A28,"NoMatchingViewException")/B33</f>
         <v>0</v>
       </c>
     </row>
@@ -12390,29 +12440,29 @@
       <c r="D4" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="18">
-        <f>COUNTIFS(C1:C28,"C1",A1:A28,"AmbiguousViewMatcherException")</f>
-        <v>5</v>
-      </c>
-      <c r="F4" s="18">
-        <f>COUNTIFS(C1:C28,"C2",A1:A28,"AmbiguousViewMatcherException")</f>
-        <v>5</v>
-      </c>
-      <c r="G4" s="18">
-        <f>COUNTIFS(C1:C28,"C3",A1:A28,"AmbiguousViewMatcherException")</f>
-        <v>4</v>
-      </c>
-      <c r="H4" s="18">
-        <f>COUNTIFS(C1:C28,"C4",A1:A28,"AmbiguousViewMatcherException")</f>
-        <v>5</v>
-      </c>
-      <c r="I4" s="18">
-        <f>COUNTIFS(C1:C28,"C5",A1:A28,"AmbiguousViewMatcherException")</f>
-        <v>4</v>
-      </c>
-      <c r="J4" s="19">
-        <f>COUNTIFS(C1:C28,"C6",A1:A28,"AmbiguousViewMatcherException")</f>
-        <v>5</v>
+      <c r="E4" s="90">
+        <f>COUNTIFS(C1:C28,"C1",A1:A28,"AmbiguousViewMatcherException")/B33</f>
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="F4" s="90">
+        <f>COUNTIFS(C1:C28,"C2",A1:A28,"AmbiguousViewMatcherException")/B33</f>
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="G4" s="90">
+        <f>COUNTIFS(C1:C28,"C3",A1:A28,"AmbiguousViewMatcherException")/B33</f>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="H4" s="90">
+        <f>COUNTIFS(C1:C28,"C4",A1:A28,"AmbiguousViewMatcherException")/B33</f>
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="I4" s="90">
+        <f>COUNTIFS(C1:C28,"C5",A1:A28,"AmbiguousViewMatcherException")/B33</f>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="J4" s="91">
+        <f>COUNTIFS(C1:C28,"C6",A1:A28,"AmbiguousViewMatcherException")/B33</f>
+        <v>0.18518518518518517</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -12702,6 +12752,11 @@
       <c r="B31">
         <f>SUM(B29:B30)</f>
         <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -12712,10 +12767,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AF542E-C13F-3949-AA4F-375C10B4CF49}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E2:J4"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12768,29 +12823,29 @@
       <c r="D2" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E2">
-        <f>COUNTIF(C1:C41,"C1")</f>
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <f>COUNTIF(C1:C41,"C2")</f>
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <f>COUNTIF(C1:C41,"C3")</f>
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <f>COUNTIF(C1:C41,"C4")</f>
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <f>COUNTIF(C1:C41,"C5")</f>
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <f>COUNTIF(C1:C41,"C6")</f>
-        <v>9</v>
+      <c r="E2" s="96">
+        <f>COUNTIF(C1:C41,"C1")/B46</f>
+        <v>0.125</v>
+      </c>
+      <c r="F2" s="96">
+        <f>COUNTIF(C1:C41,"C2")/B46</f>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="G2" s="96">
+        <f>COUNTIF(C1:C41,"C3")/B46</f>
+        <v>0.15</v>
+      </c>
+      <c r="H2" s="96">
+        <f>COUNTIF(C1:C41,"C4")/B46</f>
+        <v>0.15</v>
+      </c>
+      <c r="I2" s="96">
+        <f>COUNTIF(C1:C41,"C5")/B46</f>
+        <v>0.15</v>
+      </c>
+      <c r="J2" s="96">
+        <f>COUNTIF(C1:C41,"C6")/B46</f>
+        <v>0.22500000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12806,29 +12861,29 @@
       <c r="D3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E3">
-        <f>COUNTIFS(C1:C41,"C1",A1:A41,A1)</f>
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <f>COUNTIFS(C1:C41,"C2",A1:A41,A1)</f>
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <f>COUNTIFS(C1:C41,"C3",A1:A41,A1)</f>
-        <v>4</v>
-      </c>
-      <c r="H3" s="1">
-        <f>COUNTIFS(C1:C41,"C4",A1:A41,A1)</f>
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <f>COUNTIFS(C1:C41,"C5",A1:A41,A1)</f>
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <f>COUNTIFS(C1:C41,"C6",A1:A41,A1)</f>
-        <v>1</v>
+      <c r="E3" s="96">
+        <f>COUNTIFS(C1:C41,"C1",A1:A41,A1)/B46</f>
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="96">
+        <f>COUNTIFS(C1:C41,"C2",A1:A41,A1)/B46</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G3" s="96">
+        <f>COUNTIFS(C1:C41,"C3",A1:A41,A1)/B46</f>
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="97">
+        <f>COUNTIFS(C1:C41,"C4",A1:A41,A1)/B46</f>
+        <v>0.05</v>
+      </c>
+      <c r="I3" s="96">
+        <f>COUNTIFS(C1:C41,"C5",A1:A41,A1)/B46</f>
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="96">
+        <f>COUNTIFS(C1:C41,"C6",A1:A41,A1)/B46</f>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12844,29 +12899,29 @@
       <c r="D4" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E4">
-        <f>COUNTIFS(C1:C41,"C1",A1:A41,A5)</f>
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <f>COUNTIFS(C1:C41,"C2",A1:A41,A5)</f>
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <f>COUNTIFS(C1:C41,"C3",A1:A41,A5)</f>
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <f>COUNTIFS(C1:C41,"C4",A1:A41,A5)</f>
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <f>COUNTIFS(C1:C41,"C5",A1:A41,A5)</f>
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <f>COUNTIFS(C1:C41,"C6",A1:A41,A5)</f>
-        <v>3</v>
+      <c r="E4" s="96">
+        <f>COUNTIFS(C1:C41,"C1",A1:A41,A5)/B46</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F4" s="96">
+        <f>COUNTIFS(C1:C41,"C2",A1:A41,A5)/B46</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G4" s="96">
+        <f>COUNTIFS(C1:C41,"C3",A1:A41,A5)/B46</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="96">
+        <f>COUNTIFS(C1:C41,"C4",A1:A41,A5)/B46</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I4" s="96">
+        <f>COUNTIFS(C1:C41,"C5",A1:A41,A5)/B46</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J4" s="96">
+        <f>COUNTIFS(C1:C41,"C6",A1:A41,A5)/B46</f>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -13298,6 +13353,11 @@
       </c>
       <c r="B44" s="1">
         <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46" s="1">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -13316,10 +13376,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E68743-807A-2245-8063-C4BB37296CA9}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13369,32 +13429,32 @@
       <c r="C2" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="26">
-        <f>COUNTIF(C1:C33,"C1")</f>
-        <v>4</v>
-      </c>
-      <c r="F2" s="26">
-        <f>COUNTIF(C1:C33,"C2")</f>
-        <v>5</v>
-      </c>
-      <c r="G2" s="26">
-        <f>COUNTIF(C1:C33,"C3")</f>
-        <v>6</v>
-      </c>
-      <c r="H2" s="26">
-        <f>COUNTIF(C1:C33,"C4")</f>
-        <v>4</v>
-      </c>
-      <c r="I2" s="26">
-        <f>COUNTIF(C1:C33,"C5")</f>
-        <v>6</v>
-      </c>
-      <c r="J2" s="27">
-        <f>COUNTIF(C1:C33,"C6")</f>
-        <v>8</v>
+      <c r="E2" s="92">
+        <f>COUNTIF(C1:C33,"C1")/B38</f>
+        <v>0.125</v>
+      </c>
+      <c r="F2" s="92">
+        <f>COUNTIF(C1:C33,"C2")/B38</f>
+        <v>0.15625</v>
+      </c>
+      <c r="G2" s="92">
+        <f>COUNTIF(C1:C33,"C3")/B38</f>
+        <v>0.1875</v>
+      </c>
+      <c r="H2" s="92">
+        <f>COUNTIF(C1:C33,"C4")/B38</f>
+        <v>0.125</v>
+      </c>
+      <c r="I2" s="92">
+        <f>COUNTIF(C1:C33,"C5")/B38</f>
+        <v>0.1875</v>
+      </c>
+      <c r="J2" s="93">
+        <f>COUNTIF(C1:C33,"C6")/B38</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13407,31 +13467,31 @@
       <c r="C3" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="26">
-        <f>COUNTIFS(C1:C33,"C1",A1:A33,"NoMatchingViewException")</f>
-        <v>2</v>
-      </c>
-      <c r="F3" s="26">
-        <f>COUNTIFS(C1:C33,"C2",A1:A33,"NoMatchingViewException")</f>
-        <v>1</v>
-      </c>
-      <c r="G3" s="26">
-        <f>COUNTIFS(C1:C33,"C3",A1:A33,"NoMatchingViewException")</f>
-        <v>4</v>
-      </c>
-      <c r="H3" s="26">
-        <f>COUNTIFS(C1:C33,"C4",A1:A33,"NoMatchingViewException")</f>
-        <v>2</v>
-      </c>
-      <c r="I3" s="26">
-        <f>COUNTIFS(C1:C33,"C5",A1:A33,"NoMatchingViewException")</f>
-        <v>4</v>
-      </c>
-      <c r="J3" s="27">
-        <f>COUNTIFS(C1:C33,"C6",A1:A33,"NoMatchingViewException")</f>
+      <c r="D3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="92">
+        <f>COUNTIFS(C1:C33,"C1",A1:A33,"NoMatchingViewException")/B38</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F3" s="92">
+        <f>COUNTIFS(C1:C33,"C2",A1:A33,"NoMatchingViewException")/B38</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="G3" s="92">
+        <f>COUNTIFS(C1:C33,"C3",A1:A33,"NoMatchingViewException")/B38</f>
+        <v>0.125</v>
+      </c>
+      <c r="H3" s="92">
+        <f>COUNTIFS(C1:C33,"C4",A1:A33,"NoMatchingViewException")/B38</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="I3" s="92">
+        <f>COUNTIFS(C1:C33,"C5",A1:A33,"NoMatchingViewException")/B38</f>
+        <v>0.125</v>
+      </c>
+      <c r="J3" s="93">
+        <f>COUNTIFS(C1:C33,"C6",A1:A33,"NoMatchingViewException")/B38</f>
         <v>0</v>
       </c>
     </row>
@@ -13445,32 +13505,32 @@
       <c r="C4" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="28">
-        <f>COUNTIFS(C1:C33,"C1",A1:A33,"AmbiguousViewMatcherException")</f>
-        <v>2</v>
-      </c>
-      <c r="F4" s="28">
-        <f>COUNTIFS(C1:C33,"C2",A1:A33,"AmbiguousViewMatcherException")</f>
-        <v>4</v>
-      </c>
-      <c r="G4" s="28">
-        <f>COUNTIFS(C1:C33,"C3",A1:A33,"AmbiguousViewMatcherException")</f>
-        <v>2</v>
-      </c>
-      <c r="H4" s="28">
-        <f>COUNTIFS(C1:C33,"C4",A1:A33,"AmbiguousViewMatcherException")</f>
-        <v>2</v>
-      </c>
-      <c r="I4" s="28">
-        <f>COUNTIFS(C1:C33,"C5",A1:A33,"AmbiguousViewMatcherException")</f>
-        <v>2</v>
-      </c>
-      <c r="J4" s="29">
-        <f>COUNTIFS(C1:C33,"C6",A1:A33,"AmbiguousViewMatcherException")</f>
-        <v>8</v>
+      <c r="E4" s="94">
+        <f>COUNTIFS(C1:C33,"C1",A1:A33,"AmbiguousViewMatcherException")/B38</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F4" s="94">
+        <f>COUNTIFS(C1:C33,"C2",A1:A33,"AmbiguousViewMatcherException")/B38</f>
+        <v>0.125</v>
+      </c>
+      <c r="G4" s="94">
+        <f>COUNTIFS(C1:C33,"C3",A1:A33,"AmbiguousViewMatcherException")/B38</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H4" s="94">
+        <f>COUNTIFS(C1:C33,"C4",A1:A33,"AmbiguousViewMatcherException")/B38</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="I4" s="94">
+        <f>COUNTIFS(C1:C33,"C5",A1:A33,"AmbiguousViewMatcherException")/B38</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J4" s="95">
+        <f>COUNTIFS(C1:C33,"C6",A1:A33,"AmbiguousViewMatcherException")/B38</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -13796,7 +13856,7 @@
       <c r="A34" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="33">
+      <c r="B34" s="29">
         <v>13</v>
       </c>
     </row>
@@ -13809,11 +13869,19 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="30" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="15">
         <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>256</v>
+      </c>
+      <c r="B38">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -13832,10 +13900,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206912EB-944F-854D-A706-B96CC5AD99B5}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13855,23 +13923,23 @@
       <c r="C1" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="66" t="s">
+      <c r="D1" s="60"/>
+      <c r="E1" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="59" t="s">
         <v>116</v>
       </c>
     </row>
@@ -13885,32 +13953,32 @@
       <c r="C2" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="16">
-        <f>COUNTIF(C1:C24,"C1")</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="16">
-        <f>COUNTIF(C1:C16,"C2")</f>
-        <v>5</v>
-      </c>
-      <c r="G2" s="16">
-        <f>COUNTIF(C1:C16,"C3")</f>
-        <v>2</v>
-      </c>
-      <c r="H2" s="16">
-        <f>COUNTIF(C1:C16,"C4")</f>
-        <v>1</v>
-      </c>
-      <c r="I2" s="16">
-        <f>COUNTIF(C1:C16,"C5")</f>
-        <v>1</v>
-      </c>
-      <c r="J2" s="17">
-        <f>COUNTIF(C1:C41,"C6")</f>
-        <v>9</v>
+      <c r="E2" s="88">
+        <f>COUNTIF(C1:C24,"C1")/B29</f>
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="F2" s="88">
+        <f>COUNTIF(C1:C16,"C2")/B29</f>
+        <v>0.21739130434782608</v>
+      </c>
+      <c r="G2" s="88">
+        <f>COUNTIF(C1:C16,"C3")/B29</f>
+        <v>8.6956521739130432E-2</v>
+      </c>
+      <c r="H2" s="88">
+        <f>COUNTIF(C1:C16,"C4")/B29</f>
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="I2" s="88">
+        <f>COUNTIF(C1:C16,"C5")/B29</f>
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="J2" s="89">
+        <f>COUNTIF(C1:C41,"C6")/B29</f>
+        <v>0.39130434782608697</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13923,32 +13991,32 @@
       <c r="C3" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="16">
-        <f>COUNTIFS(C1:C24,"C1",A1:A24,"NoMatchingViewException")</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="16">
-        <f>COUNTIFS(C1:C24,"C2",A1:A24,"NoMatchingViewException")</f>
-        <v>1</v>
-      </c>
-      <c r="G3" s="16">
-        <f>COUNTIFS(C1:C24,"C3",A1:A24,"NoMatchingViewException")</f>
-        <v>3</v>
-      </c>
-      <c r="H3" s="16">
-        <f>COUNTIFS(C1:C24,"C4",A1:A24,"NoMatchingViewException")</f>
-        <v>1</v>
-      </c>
-      <c r="I3" s="16">
-        <f>COUNTIFS(C1:C24,"C5",A1:A24,"NoMatchingViewException")</f>
-        <v>1</v>
-      </c>
-      <c r="J3" s="17">
-        <f>COUNTIFS(C1:C24,"C6",A1:A24,"NoMatchingViewException")</f>
-        <v>1</v>
+      <c r="D3" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="88">
+        <f>COUNTIFS(C1:C24,"C1",A1:A24,"NoMatchingViewException")/B29</f>
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="F3" s="88">
+        <f>COUNTIFS(C1:C24,"C2",A1:A24,"NoMatchingViewException")/B29</f>
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="G3" s="88">
+        <f>COUNTIFS(C1:C24,"C3",A1:A24,"NoMatchingViewException")/B29</f>
+        <v>0.13043478260869565</v>
+      </c>
+      <c r="H3" s="88">
+        <f>COUNTIFS(C1:C24,"C4",A1:A24,"NoMatchingViewException")/B29</f>
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="I3" s="88">
+        <f>COUNTIFS(C1:C24,"C5",A1:A24,"NoMatchingViewException")/B29</f>
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="J3" s="89">
+        <f>COUNTIFS(C1:C24,"C6",A1:A24,"NoMatchingViewException")/B29</f>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -13961,32 +14029,32 @@
       <c r="C4" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="18">
-        <f>COUNTIFS(C1:C24,"C1",A1:A24,"AmbiguousViewMatcherException")</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="18">
-        <f>COUNTIFS(C1:C24,"C2",A1:A24,"AmbiguousViewMatcherException")</f>
-        <v>7</v>
-      </c>
-      <c r="G4" s="18">
-        <f>COUNTIFS(C1:C24,"C3",A1:A24,"AmbiguousViewMatcherException")</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="18">
-        <f>COUNTIFS(C1:C24,"C4",A1:A24,"AmbiguousViewMatcherException")</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="18">
-        <f>COUNTIFS(C1:C24,"C5",A1:A24,"AmbiguousViewMatcherException")</f>
-        <v>1</v>
-      </c>
-      <c r="J4" s="19">
-        <f>COUNTIFS(C1:C24,"C6",A1:A24,"AmbiguousViewMatcherException")</f>
-        <v>8</v>
+      <c r="E4" s="90">
+        <f>COUNTIFS(C1:C24,"C1",A1:A24,"AmbiguousViewMatcherException")/B29</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="90">
+        <f>COUNTIFS(C1:C24,"C2",A1:A24,"AmbiguousViewMatcherException")/B29</f>
+        <v>0.30434782608695654</v>
+      </c>
+      <c r="G4" s="90">
+        <f>COUNTIFS(C1:C24,"C3",A1:A24,"AmbiguousViewMatcherException")/B29</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="90">
+        <f>COUNTIFS(C1:C24,"C4",A1:A24,"AmbiguousViewMatcherException")/B29</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="90">
+        <f>COUNTIFS(C1:C24,"C5",A1:A24,"AmbiguousViewMatcherException")/B29</f>
+        <v>4.3478260869565216E-2</v>
+      </c>
+      <c r="J4" s="91">
+        <f>COUNTIFS(C1:C24,"C6",A1:A24,"AmbiguousViewMatcherException")/B29</f>
+        <v>0.34782608695652173</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -14231,6 +14299,14 @@
       </c>
       <c r="B27">
         <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B29" s="87">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -14246,10 +14322,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2DF7DC1-906F-8847-A0B3-CD943C8D1315}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14258,69 +14334,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="72"/>
-      <c r="B1" s="76" t="s">
+      <c r="A1" s="64"/>
+      <c r="B1" s="68" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="76" t="s">
+      <c r="E1" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="76" t="s">
+      <c r="F1" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="69" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="65" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="79">
         <v>31</v>
       </c>
-      <c r="C2" s="59">
+      <c r="C2" s="79">
         <v>39</v>
       </c>
-      <c r="D2" s="59">
+      <c r="D2" s="79">
         <v>39</v>
       </c>
-      <c r="E2" s="59">
+      <c r="E2" s="79">
         <v>32</v>
       </c>
-      <c r="F2" s="59">
+      <c r="F2" s="79">
         <v>39</v>
       </c>
-      <c r="G2" s="60">
+      <c r="G2" s="80">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="59">
+      <c r="A3" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="79">
         <v>19</v>
       </c>
-      <c r="C3" s="59">
+      <c r="C3" s="79">
         <v>11</v>
       </c>
-      <c r="D3" s="59">
+      <c r="D3" s="79">
         <v>32</v>
       </c>
-      <c r="E3" s="59">
+      <c r="E3" s="79">
         <v>19</v>
       </c>
-      <c r="F3" s="59">
+      <c r="F3" s="79">
         <v>31</v>
       </c>
-      <c r="G3" s="60">
+      <c r="G3" s="80">
         <v>6</v>
       </c>
       <c r="H3">
@@ -14329,30 +14405,138 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="61">
+      <c r="B4" s="81">
         <v>10</v>
       </c>
-      <c r="C4" s="61">
+      <c r="C4" s="81">
         <v>26</v>
       </c>
-      <c r="D4" s="61">
+      <c r="D4" s="81">
         <v>6</v>
       </c>
-      <c r="E4" s="61">
+      <c r="E4" s="81">
         <v>10</v>
       </c>
-      <c r="F4" s="61">
+      <c r="F4" s="81">
         <v>8</v>
       </c>
-      <c r="G4" s="62">
+      <c r="G4" s="82">
         <v>34</v>
       </c>
       <c r="H4">
         <f>SUM(B4:G4)</f>
         <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="64"/>
+      <c r="B6" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="69" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="83">
+        <f>B2/70</f>
+        <v>0.44285714285714284</v>
+      </c>
+      <c r="C7" s="83">
+        <f>C2/70</f>
+        <v>0.55714285714285716</v>
+      </c>
+      <c r="D7" s="83">
+        <f>D2/70</f>
+        <v>0.55714285714285716</v>
+      </c>
+      <c r="E7" s="83">
+        <f>E2/70</f>
+        <v>0.45714285714285713</v>
+      </c>
+      <c r="F7" s="83">
+        <f t="shared" ref="F7:G7" si="0">F2/70</f>
+        <v>0.55714285714285716</v>
+      </c>
+      <c r="G7" s="84">
+        <f t="shared" si="0"/>
+        <v>0.6428571428571429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="83">
+        <f t="shared" ref="B8:G9" si="1">B3/70</f>
+        <v>0.27142857142857141</v>
+      </c>
+      <c r="C8" s="83">
+        <f t="shared" si="1"/>
+        <v>0.15714285714285714</v>
+      </c>
+      <c r="D8" s="83">
+        <f t="shared" si="1"/>
+        <v>0.45714285714285713</v>
+      </c>
+      <c r="E8" s="83">
+        <f t="shared" si="1"/>
+        <v>0.27142857142857141</v>
+      </c>
+      <c r="F8" s="83">
+        <f t="shared" si="1"/>
+        <v>0.44285714285714284</v>
+      </c>
+      <c r="G8" s="84">
+        <f t="shared" si="1"/>
+        <v>8.5714285714285715E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="85">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="C9" s="85">
+        <f t="shared" si="1"/>
+        <v>0.37142857142857144</v>
+      </c>
+      <c r="D9" s="85">
+        <f t="shared" si="1"/>
+        <v>8.5714285714285715E-2</v>
+      </c>
+      <c r="E9" s="85">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="F9" s="85">
+        <f t="shared" si="1"/>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="G9" s="86">
+        <f t="shared" si="1"/>
+        <v>0.48571428571428571</v>
       </c>
     </row>
   </sheetData>
@@ -14375,100 +14559,131 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7255DB6A-00B4-B34A-9D73-A7DCE2821CD8}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="70" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="71" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="71" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="80" t="s">
+      <c r="D1" s="77" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="81">
+      <c r="B2" s="74">
         <v>70</v>
       </c>
-      <c r="C2" s="81">
+      <c r="C2" s="74">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="80" t="s">
+      <c r="D2" s="78">
+        <f>C2/B2</f>
+        <v>0.48571428571428571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="81">
+      <c r="B3" s="74">
         <v>70</v>
       </c>
-      <c r="C3" s="81">
+      <c r="C3" s="74">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="80" t="s">
+      <c r="D3" s="78">
+        <f t="shared" ref="D3:D8" si="0">C3/B3</f>
+        <v>0.62857142857142856</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="81">
+      <c r="B4" s="74">
         <v>70</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="74">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="80" t="s">
+      <c r="D4" s="78">
+        <f t="shared" si="0"/>
+        <v>0.6428571428571429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="81">
+      <c r="B5" s="74">
         <v>70</v>
       </c>
-      <c r="C5" s="81">
+      <c r="C5" s="74">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="80" t="s">
+      <c r="D5" s="78">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="72" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="81">
+      <c r="B6" s="74">
         <v>70</v>
       </c>
-      <c r="C6" s="81">
+      <c r="C6" s="74">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="80" t="s">
+      <c r="D6" s="78">
+        <f t="shared" si="0"/>
+        <v>0.65714285714285714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="81">
+      <c r="B7" s="74">
         <v>70</v>
       </c>
-      <c r="C7" s="81">
+      <c r="C7" s="74">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="17">
-      <c r="A8" s="82" t="s">
+      <c r="D7" s="78">
+        <f>C7/B7</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17">
+      <c r="A8" s="73" t="s">
         <v>253</v>
       </c>
-      <c r="B8" s="83">
+      <c r="B8" s="75">
         <v>420</v>
       </c>
-      <c r="C8" s="83">
+      <c r="C8" s="75">
         <v>253</v>
+      </c>
+      <c r="D8" s="76">
+        <f t="shared" si="0"/>
+        <v>0.60238095238095235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>